<commit_message>
Added some code. in public methos.
</commit_message>
<xml_diff>
--- a/ExcelPracticalTask/wwwroot/inevtory task.xlsx
+++ b/ExcelPracticalTask/wwwroot/inevtory task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soumy.oza\source\repos\ExcelPracticalTaskWeb\ExcelPracticalTask\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F9B295-B6A3-4ACF-9726-03B3228A3727}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F3B61C-030A-4440-9FC8-155BE8FBD1A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{3D136046-B5E0-4C38-A60F-BC44D394FBC6}"/>
   </bookViews>
@@ -424,7 +424,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="4">
-        <v>44947</v>
+        <v>44978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added closing qty part.
</commit_message>
<xml_diff>
--- a/ExcelPracticalTask/wwwroot/inevtory task.xlsx
+++ b/ExcelPracticalTask/wwwroot/inevtory task.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soumy.oza\source\repos\ExcelPracticalTaskWeb\ExcelPracticalTask\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F3B61C-030A-4440-9FC8-155BE8FBD1A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE36C0F-AE69-49D0-AC19-AF283E1EB05F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{3D136046-B5E0-4C38-A60F-BC44D394FBC6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Event 1 =  Purchase , 2 = Sale</t>
   </si>
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F076C7FB-B24D-4C54-A0E9-AD398E32DE31}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,24 @@
         <v>35</v>
       </c>
       <c r="E7" s="4">
-        <v>44978</v>
+        <v>44947</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>55</v>
+      </c>
+      <c r="D8" s="3">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4">
+        <v>44948</v>
       </c>
     </row>
   </sheetData>

</xml_diff>